<commit_message>
emails de jeudi pret
</commit_message>
<xml_diff>
--- a/data/contacts/ORANGE - contacts.xlsx
+++ b/data/contacts/ORANGE - contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8010174\Desktop\projects\Lettre de Motivation adapter\data\contacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D93E02A-AE32-47E8-ADF0-F4675B197DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216144DD-7314-495C-8E46-3B144E5B0D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,9 +210,6 @@
     <t>sara.madani@orange.com</t>
   </si>
   <si>
-    <t>Cloud &amp; Data Engineer, GCP</t>
-  </si>
-  <si>
     <t>Arcueil, Île-de-France, France</t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>Nathalie CHEYMOL</t>
+  </si>
+  <si>
+    <t>Cloud &amp; Data Engineer</t>
   </si>
 </sst>
 </file>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,10 +944,10 @@
         <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>11</v>
@@ -955,19 +955,19 @@
     </row>
     <row r="15" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>11</v>
@@ -975,19 +975,19 @@
     </row>
     <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>24</v>
@@ -995,19 +995,19 @@
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>24</v>
@@ -1015,19 +1015,19 @@
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>11</v>
@@ -1035,16 +1035,16 @@
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>15</v>
@@ -1055,19 +1055,19 @@
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>11</v>
@@ -1075,19 +1075,19 @@
     </row>
     <row r="21" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>24</v>
@@ -1095,16 +1095,16 @@
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>15</v>

</xml_diff>